<commit_message>
added inner and outer list makings
</commit_message>
<xml_diff>
--- a/outputs/complete_lists/Older Adults/OA S033.xlsx
+++ b/outputs/complete_lists/Older Adults/OA S033.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amuller\Desktop\Alana\UA\R_projects\inflatable-project\outputs\complete_lists\Older Adults\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5807AB4-095E-47B4-8368-F5F96178C325}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A38873-DC86-4730-AFD5-7AD2F8BBEB56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39920" yWindow="470" windowWidth="25910" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39290" yWindow="910" windowWidth="27940" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ten_lists" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="140">
   <si>
     <t>DD_#</t>
   </si>
@@ -431,6 +431,15 @@
   </si>
   <si>
     <t>S033</t>
+  </si>
+  <si>
+    <t>start SD</t>
+  </si>
+  <si>
+    <t>start DD</t>
+  </si>
+  <si>
+    <t>didn't do this trial</t>
   </si>
 </sst>
 </file>
@@ -1287,10 +1296,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1314,10 +1323,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
-        <v>132</v>
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>137</v>
       </c>
       <c r="I3" t="s">
-        <v>133</v>
+        <v>135</v>
+      </c>
+      <c r="K3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
@@ -1460,8 +1475,14 @@
       <c r="C10" t="s">
         <v>133</v>
       </c>
+      <c r="E10" t="s">
+        <v>138</v>
+      </c>
       <c r="I10" t="s">
         <v>134</v>
+      </c>
+      <c r="K10" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
@@ -1600,15 +1621,21 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C17" t="s">
-        <v>134</v>
+        <v>132</v>
+      </c>
+      <c r="E17" t="s">
+        <v>137</v>
       </c>
       <c r="I17" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+      <c r="K17" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>3</v>
       </c>
@@ -1640,7 +1667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1666,7 +1693,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1692,7 +1719,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
@@ -1718,7 +1745,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1744,15 +1771,21 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C24" t="s">
         <v>135</v>
       </c>
+      <c r="E24" t="s">
+        <v>138</v>
+      </c>
       <c r="I24" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>4</v>
       </c>
@@ -1783,8 +1816,11 @@
       <c r="K25" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="M25" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1810,7 +1846,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
@@ -1836,7 +1872,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1862,7 +1898,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
@@ -1888,15 +1924,21 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="C31" t="s">
         <v>132</v>
       </c>
+      <c r="E31" t="s">
+        <v>138</v>
+      </c>
       <c r="I31" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K31" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>5</v>
       </c>
@@ -1926,6 +1968,9 @@
       </c>
       <c r="K32" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="M32" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.35">

</xml_diff>